<commit_message>
Update Gitignore and NUTS regions
</commit_message>
<xml_diff>
--- a/NUTS_regions_germany.xlsx
+++ b/NUTS_regions_germany.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bbhberatung-my.sharepoint.com/personal/heinrich_boeing_bbh-beratung_de/Documents/Github/udacity-data_analyst-project2-data_wrangling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9847790D-B483-4F95-9011-80A103ABA44F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{9847790D-B483-4F95-9011-80A103ABA44F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F1273C9-4543-4A03-97C7-C7BED3F6C3AD}"/>
   <bookViews>
-    <workbookView xWindow="14317" yWindow="0" windowWidth="14565" windowHeight="17363" xr2:uid="{F4D20D3F-8A9C-44FB-98C9-C61A0AA8FCEF}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="12735" xr2:uid="{F4D20D3F-8A9C-44FB-98C9-C61A0AA8FCEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>DE1</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>Thüringen</t>
+  </si>
+  <si>
+    <t>NUTS1</t>
+  </si>
+  <si>
+    <t>State</t>
   </si>
 </sst>
 </file>
@@ -483,139 +489,147 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEB3C672-5B86-49D9-B0FC-B5D712393E88}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
         <v>30</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>